<commit_message>
Changed SummaryStats to only output maxes that are detected. Added TableProcessor to run all of the files without haveing to open them individually.
</commit_message>
<xml_diff>
--- a/Tables/Alluvial- Appendix.xlsx
+++ b/Tables/Alluvial- Appendix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Alluvial for Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Alluvial Exhibit" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alluvial for Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alluvial Exhibit" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="V6" s="1" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="W6" s="1" t="inlineStr">
         <is>
-          <t>2008-05-22</t>
+          <t>2008-02-11</t>
         </is>
       </c>
       <c r="X6" s="1" t="inlineStr">
@@ -1393,12 +1393,12 @@
       </c>
       <c r="V7" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W7" s="1" t="inlineStr">
         <is>
-          <t>2008-11-13</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X7" s="1" t="inlineStr">
@@ -2265,12 +2265,12 @@
       </c>
       <c r="V13" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>6.69</t>
         </is>
       </c>
       <c r="W13" s="1" t="inlineStr">
         <is>
-          <t>1996-03-05</t>
+          <t>2010-07-06</t>
         </is>
       </c>
       <c r="X13" s="1" t="inlineStr">
@@ -2405,12 +2405,12 @@
       </c>
       <c r="V14" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>4.81</t>
         </is>
       </c>
       <c r="W14" s="1" t="inlineStr">
         <is>
-          <t>2008-02-21</t>
+          <t>2010-07-07</t>
         </is>
       </c>
       <c r="X14" s="1" t="inlineStr">
@@ -2557,12 +2557,12 @@
       </c>
       <c r="V15" s="1" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W15" s="1" t="inlineStr">
         <is>
-          <t>1998-05-27</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X15" s="1" t="inlineStr">
@@ -2689,12 +2689,12 @@
       </c>
       <c r="V16" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>4.69</t>
         </is>
       </c>
       <c r="W16" s="1" t="inlineStr">
         <is>
-          <t>2008-02-06</t>
+          <t>2010-07-08</t>
         </is>
       </c>
       <c r="X16" s="1" t="inlineStr">
@@ -2961,12 +2961,12 @@
       </c>
       <c r="V18" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.63</t>
         </is>
       </c>
       <c r="W18" s="1" t="inlineStr">
         <is>
-          <t>2008-02-06</t>
+          <t>2010-07-09</t>
         </is>
       </c>
       <c r="X18" s="1" t="inlineStr">
@@ -3089,12 +3089,12 @@
       </c>
       <c r="V19" s="1" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="W19" s="1" t="inlineStr">
         <is>
-          <t>1998-08-26</t>
+          <t>2007-03-13</t>
         </is>
       </c>
       <c r="X19" s="1" t="inlineStr">
@@ -3233,12 +3233,12 @@
       </c>
       <c r="V20" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.26</t>
         </is>
       </c>
       <c r="W20" s="1" t="inlineStr">
         <is>
-          <t>2008-01-16</t>
+          <t>2013-06-05</t>
         </is>
       </c>
       <c r="X20" s="1" t="inlineStr">
@@ -3361,12 +3361,12 @@
       </c>
       <c r="V21" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W21" s="1" t="inlineStr">
         <is>
-          <t>2011-03-07</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X21" s="1" t="inlineStr">
@@ -3509,12 +3509,12 @@
       </c>
       <c r="V22" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="W22" s="1" t="inlineStr">
         <is>
-          <t>2011-03-08</t>
+          <t>2006-08-03</t>
         </is>
       </c>
       <c r="X22" s="1" t="inlineStr">
@@ -3653,12 +3653,12 @@
       </c>
       <c r="V23" s="1" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>0.885</t>
         </is>
       </c>
       <c r="W23" s="1" t="inlineStr">
         <is>
-          <t>1997-06-18</t>
+          <t>2003-07-09</t>
         </is>
       </c>
       <c r="X23" s="1" t="inlineStr">
@@ -4077,12 +4077,12 @@
       </c>
       <c r="V26" s="1" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="W26" s="1" t="inlineStr">
         <is>
-          <t>1996-11-13</t>
+          <t>2007-07-23</t>
         </is>
       </c>
       <c r="X26" s="1" t="inlineStr">
@@ -4229,12 +4229,12 @@
       </c>
       <c r="V27" s="1" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W27" s="1" t="inlineStr">
         <is>
-          <t>1996-07-29</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X27" s="1" t="inlineStr">
@@ -4357,12 +4357,12 @@
       </c>
       <c r="V28" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="W28" s="1" t="inlineStr">
         <is>
-          <t>2009-07-14</t>
+          <t>2007-07-19</t>
         </is>
       </c>
       <c r="X28" s="1" t="inlineStr">
@@ -4485,12 +4485,12 @@
       </c>
       <c r="V29" s="1" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="W29" s="1" t="inlineStr">
         <is>
-          <t>1998-08-31</t>
+          <t>2007-08-03</t>
         </is>
       </c>
       <c r="X29" s="1" t="inlineStr">
@@ -4633,12 +4633,12 @@
       </c>
       <c r="V30" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="W30" s="1" t="inlineStr">
         <is>
-          <t>2009-07-14</t>
+          <t>2005-05-10</t>
         </is>
       </c>
       <c r="X30" s="1" t="inlineStr">
@@ -4781,12 +4781,12 @@
       </c>
       <c r="V31" s="1" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>1.02</t>
         </is>
       </c>
       <c r="W31" s="1" t="inlineStr">
         <is>
-          <t>1996-07-10</t>
+          <t>2003-07-09</t>
         </is>
       </c>
       <c r="X31" s="1" t="inlineStr">
@@ -5085,12 +5085,12 @@
       </c>
       <c r="V33" s="1" t="inlineStr">
         <is>
-          <t>7.04</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="W33" s="1" t="inlineStr">
         <is>
-          <t>2009-07-20</t>
+          <t>2007-08-02</t>
         </is>
       </c>
       <c r="X33" s="1" t="inlineStr">
@@ -5233,12 +5233,12 @@
       </c>
       <c r="V34" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>6.72</t>
         </is>
       </c>
       <c r="W34" s="1" t="inlineStr">
         <is>
-          <t>2008-03-04</t>
+          <t>2010-02-22</t>
         </is>
       </c>
       <c r="X34" s="1" t="inlineStr">
@@ -5377,12 +5377,12 @@
       </c>
       <c r="V35" s="1" t="inlineStr">
         <is>
-          <t>10.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="W35" s="1" t="inlineStr">
         <is>
-          <t>2007-03-28</t>
+          <t>2008-06-17</t>
         </is>
       </c>
       <c r="X35" s="1" t="inlineStr">
@@ -5525,12 +5525,12 @@
       </c>
       <c r="V36" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="W36" s="1" t="inlineStr">
         <is>
-          <t>2008-03-03</t>
+          <t>2008-06-16</t>
         </is>
       </c>
       <c r="X36" s="1" t="inlineStr">
@@ -5677,12 +5677,12 @@
       </c>
       <c r="V37" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="W37" s="1" t="inlineStr">
         <is>
-          <t>2007-12-18</t>
+          <t>2006-12-11</t>
         </is>
       </c>
       <c r="X37" s="1" t="inlineStr">
@@ -5829,12 +5829,12 @@
       </c>
       <c r="V38" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.56</t>
         </is>
       </c>
       <c r="W38" s="1" t="inlineStr">
         <is>
-          <t>2008-06-23</t>
+          <t>2010-06-07</t>
         </is>
       </c>
       <c r="X38" s="1" t="inlineStr">
@@ -5981,12 +5981,12 @@
       </c>
       <c r="V39" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W39" s="1" t="inlineStr">
         <is>
-          <t>2008-06-09</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X39" s="1" t="inlineStr">
@@ -6133,7 +6133,7 @@
       </c>
       <c r="V40" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="W40" s="1" t="inlineStr">
@@ -6285,12 +6285,12 @@
       </c>
       <c r="V41" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W41" s="1" t="inlineStr">
         <is>
-          <t>2008-06-22</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X41" s="1" t="inlineStr">
@@ -6437,12 +6437,12 @@
       </c>
       <c r="V42" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="W42" s="1" t="inlineStr">
         <is>
-          <t>2008-06-25</t>
+          <t>2008-12-18</t>
         </is>
       </c>
       <c r="X42" s="1" t="inlineStr">
@@ -6589,12 +6589,12 @@
       </c>
       <c r="V43" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.74</t>
         </is>
       </c>
       <c r="W43" s="1" t="inlineStr">
         <is>
-          <t>2008-06-22</t>
+          <t>2009-09-14</t>
         </is>
       </c>
       <c r="X43" s="1" t="inlineStr">
@@ -6741,12 +6741,12 @@
       </c>
       <c r="V44" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="W44" s="1" t="inlineStr">
         <is>
-          <t>2008-06-25</t>
+          <t>2008-09-17</t>
         </is>
       </c>
       <c r="X44" s="1" t="inlineStr">
@@ -6881,12 +6881,12 @@
       </c>
       <c r="V45" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="W45" s="1" t="inlineStr">
         <is>
-          <t>1999-03-26</t>
+          <t>2005-08-24</t>
         </is>
       </c>
       <c r="X45" s="1" t="inlineStr">
@@ -7017,12 +7017,12 @@
       </c>
       <c r="V46" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="W46" s="1" t="inlineStr">
         <is>
-          <t>2008-03-07</t>
+          <t>2007-06-25</t>
         </is>
       </c>
       <c r="X46" s="1" t="inlineStr">
@@ -7153,12 +7153,12 @@
       </c>
       <c r="V47" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="W47" s="1" t="inlineStr">
         <is>
-          <t>2008-03-18</t>
+          <t>2007-12-07</t>
         </is>
       </c>
       <c r="X47" s="1" t="inlineStr">
@@ -7305,12 +7305,12 @@
       </c>
       <c r="V48" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="W48" s="1" t="inlineStr">
         <is>
-          <t>2010-06-02</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="X48" s="1" t="inlineStr">
@@ -7652,12 +7652,12 @@
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>5/22/08</t>
+          <t>2/11/08</t>
         </is>
       </c>
     </row>
@@ -7694,12 +7694,12 @@
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>11/13/08</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
@@ -7946,12 +7946,12 @@
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>6.69</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
-          <t>3/5/96</t>
+          <t>7/6/10</t>
         </is>
       </c>
     </row>
@@ -7988,12 +7988,12 @@
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4.81</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>2/21/08</t>
+          <t>7/7/10</t>
         </is>
       </c>
     </row>
@@ -8030,12 +8030,12 @@
       </c>
       <c r="G18" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H18" s="1" t="inlineStr">
         <is>
-          <t>5/27/98</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
@@ -8072,12 +8072,12 @@
       </c>
       <c r="G19" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4.69</t>
         </is>
       </c>
       <c r="H19" s="1" t="inlineStr">
         <is>
-          <t>2/6/08</t>
+          <t>7/8/10</t>
         </is>
       </c>
     </row>
@@ -8156,12 +8156,12 @@
       </c>
       <c r="G21" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5.63</t>
         </is>
       </c>
       <c r="H21" s="1" t="inlineStr">
         <is>
-          <t>2/6/08</t>
+          <t>7/9/10</t>
         </is>
       </c>
     </row>
@@ -8198,12 +8198,12 @@
       </c>
       <c r="G22" s="1" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="H22" s="1" t="inlineStr">
         <is>
-          <t>8/26/98</t>
+          <t>3/13/07</t>
         </is>
       </c>
     </row>
@@ -8248,12 +8248,12 @@
       </c>
       <c r="G24" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2.26</t>
         </is>
       </c>
       <c r="H24" s="1" t="inlineStr">
         <is>
-          <t>1/16/08</t>
+          <t>6/5/13</t>
         </is>
       </c>
     </row>
@@ -8290,12 +8290,12 @@
       </c>
       <c r="G25" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H25" s="1" t="inlineStr">
         <is>
-          <t>3/7/11</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
@@ -8332,12 +8332,12 @@
       </c>
       <c r="G26" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="H26" s="1" t="inlineStr">
         <is>
-          <t>3/8/11</t>
+          <t>8/3/06</t>
         </is>
       </c>
     </row>
@@ -8374,12 +8374,12 @@
       </c>
       <c r="G27" s="1" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>0.885</t>
         </is>
       </c>
       <c r="H27" s="1" t="inlineStr">
         <is>
-          <t>6/18/97</t>
+          <t>7/9/03</t>
         </is>
       </c>
     </row>
@@ -8500,12 +8500,12 @@
       </c>
       <c r="G30" s="1" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="H30" s="1" t="inlineStr">
         <is>
-          <t>11/13/96</t>
+          <t>7/23/07</t>
         </is>
       </c>
     </row>
@@ -8542,12 +8542,12 @@
       </c>
       <c r="G31" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H31" s="1" t="inlineStr">
         <is>
-          <t>7/29/96</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
@@ -8584,12 +8584,12 @@
       </c>
       <c r="G32" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="H32" s="1" t="inlineStr">
         <is>
-          <t>7/14/09</t>
+          <t>7/19/07</t>
         </is>
       </c>
     </row>
@@ -8626,12 +8626,12 @@
       </c>
       <c r="G33" s="1" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="H33" s="1" t="inlineStr">
         <is>
-          <t>8/31/98</t>
+          <t>8/3/07</t>
         </is>
       </c>
     </row>
@@ -8668,12 +8668,12 @@
       </c>
       <c r="G34" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="H34" s="1" t="inlineStr">
         <is>
-          <t>7/14/09</t>
+          <t>5/10/05</t>
         </is>
       </c>
     </row>
@@ -8710,12 +8710,12 @@
       </c>
       <c r="G35" s="1" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>1.02</t>
         </is>
       </c>
       <c r="H35" s="1" t="inlineStr">
         <is>
-          <t>7/10/96</t>
+          <t>7/9/03</t>
         </is>
       </c>
     </row>
@@ -8794,12 +8794,12 @@
       </c>
       <c r="G37" s="1" t="inlineStr">
         <is>
-          <t>7.04</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="H37" s="1" t="inlineStr">
         <is>
-          <t>7/20/09</t>
+          <t>8/2/07</t>
         </is>
       </c>
     </row>
@@ -8836,12 +8836,12 @@
       </c>
       <c r="G38" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>6.72</t>
         </is>
       </c>
       <c r="H38" s="1" t="inlineStr">
         <is>
-          <t>3/4/08</t>
+          <t>2/22/10</t>
         </is>
       </c>
     </row>
@@ -8874,12 +8874,12 @@
       </c>
       <c r="G39" s="1" t="inlineStr">
         <is>
-          <t>10.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="H39" s="1" t="inlineStr">
         <is>
-          <t>3/28/07</t>
+          <t>6/17/08</t>
         </is>
       </c>
     </row>
@@ -8916,12 +8916,12 @@
       </c>
       <c r="G40" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="H40" s="1" t="inlineStr">
         <is>
-          <t>3/3/08</t>
+          <t>6/16/08</t>
         </is>
       </c>
     </row>
@@ -8958,12 +8958,12 @@
       </c>
       <c r="G41" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="H41" s="1" t="inlineStr">
         <is>
-          <t>12/18/07</t>
+          <t>12/11/06</t>
         </is>
       </c>
     </row>
@@ -9000,12 +9000,12 @@
       </c>
       <c r="G42" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5.56</t>
         </is>
       </c>
       <c r="H42" s="1" t="inlineStr">
         <is>
-          <t>6/23/08</t>
+          <t>6/7/10</t>
         </is>
       </c>
     </row>
@@ -9042,12 +9042,12 @@
       </c>
       <c r="G43" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H43" s="1" t="inlineStr">
         <is>
-          <t>6/9/08</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
@@ -9084,7 +9084,7 @@
       </c>
       <c r="G44" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="H44" s="1" t="inlineStr">
@@ -9126,12 +9126,12 @@
       </c>
       <c r="G45" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H45" s="1" t="inlineStr">
         <is>
-          <t>6/22/08</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
@@ -9168,12 +9168,12 @@
       </c>
       <c r="G46" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H46" s="1" t="inlineStr">
         <is>
-          <t>6/25/08</t>
+          <t>12/18/08</t>
         </is>
       </c>
     </row>
@@ -9210,12 +9210,12 @@
       </c>
       <c r="G47" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2.74</t>
         </is>
       </c>
       <c r="H47" s="1" t="inlineStr">
         <is>
-          <t>6/22/08</t>
+          <t>9/14/09</t>
         </is>
       </c>
     </row>
@@ -9252,12 +9252,12 @@
       </c>
       <c r="G48" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H48" s="1" t="inlineStr">
         <is>
-          <t>6/25/08</t>
+          <t>9/17/08</t>
         </is>
       </c>
     </row>
@@ -9294,12 +9294,12 @@
       </c>
       <c r="G49" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H49" s="1" t="inlineStr">
         <is>
-          <t>3/26/99</t>
+          <t>8/24/05</t>
         </is>
       </c>
     </row>
@@ -9336,12 +9336,12 @@
       </c>
       <c r="G50" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="H50" s="1" t="inlineStr">
         <is>
-          <t>3/7/08</t>
+          <t>6/25/07</t>
         </is>
       </c>
     </row>
@@ -9378,12 +9378,12 @@
       </c>
       <c r="G51" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="H51" s="1" t="inlineStr">
         <is>
-          <t>3/18/08</t>
+          <t>12/7/07</t>
         </is>
       </c>
     </row>
@@ -9420,12 +9420,12 @@
       </c>
       <c r="G52" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H52" s="1" t="inlineStr">
         <is>
-          <t>6/2/10</t>
+          <t>NA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed SummaryStats so that the last value has to be a detected result.
</commit_message>
<xml_diff>
--- a/Tables/Alluvial- Appendix.xlsx
+++ b/Tables/Alluvial- Appendix.xlsx
@@ -1267,7 +1267,7 @@
       </c>
       <c r="X6" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="Y6" s="1" t="inlineStr">
@@ -1403,12 +1403,12 @@
       </c>
       <c r="X7" s="1" t="inlineStr">
         <is>
-          <t>2.38</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y7" s="1" t="inlineStr">
         <is>
-          <t>2009-05-06</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z7" s="1" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="X8" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="Y8" s="1" t="inlineStr">
         <is>
-          <t>2009-08-06</t>
+          <t>2008-11-06</t>
         </is>
       </c>
       <c r="Z8" s="1" t="inlineStr">
@@ -2567,12 +2567,12 @@
       </c>
       <c r="X15" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y15" s="1" t="inlineStr">
         <is>
-          <t>1999-04-14</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z15" s="1" t="inlineStr">
@@ -3371,12 +3371,12 @@
       </c>
       <c r="X21" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y21" s="1" t="inlineStr">
         <is>
-          <t>2011-03-07</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z21" s="1" t="inlineStr">
@@ -3519,12 +3519,12 @@
       </c>
       <c r="X22" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="Y22" s="1" t="inlineStr">
         <is>
-          <t>2011-03-08</t>
+          <t>2008-08-29</t>
         </is>
       </c>
       <c r="Z22" s="1" t="inlineStr">
@@ -3955,12 +3955,12 @@
       </c>
       <c r="X25" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="Y25" s="1" t="inlineStr">
         <is>
-          <t>2009-07-16</t>
+          <t>2008-08-27</t>
         </is>
       </c>
       <c r="Z25" s="1" t="inlineStr">
@@ -4239,12 +4239,12 @@
       </c>
       <c r="X27" s="1" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y27" s="1" t="inlineStr">
         <is>
-          <t>2001-04-05</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z27" s="1" t="inlineStr">
@@ -4367,12 +4367,12 @@
       </c>
       <c r="X28" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Y28" s="1" t="inlineStr">
         <is>
-          <t>2009-07-14</t>
+          <t>2007-07-19</t>
         </is>
       </c>
       <c r="Z28" s="1" t="inlineStr">
@@ -4643,12 +4643,12 @@
       </c>
       <c r="X30" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="Y30" s="1" t="inlineStr">
         <is>
-          <t>2011-03-07</t>
+          <t>2005-05-10</t>
         </is>
       </c>
       <c r="Z30" s="1" t="inlineStr">
@@ -4791,12 +4791,12 @@
       </c>
       <c r="X31" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.509</t>
         </is>
       </c>
       <c r="Y31" s="1" t="inlineStr">
         <is>
-          <t>2005-05-05</t>
+          <t>2004-06-03</t>
         </is>
       </c>
       <c r="Z31" s="1" t="inlineStr">
@@ -5095,12 +5095,12 @@
       </c>
       <c r="X33" s="1" t="inlineStr">
         <is>
-          <t>7.04</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="Y33" s="1" t="inlineStr">
         <is>
-          <t>2009-07-20</t>
+          <t>2007-08-02</t>
         </is>
       </c>
       <c r="Z33" s="1" t="inlineStr">
@@ -5535,12 +5535,12 @@
       </c>
       <c r="X36" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.78</t>
         </is>
       </c>
       <c r="Y36" s="1" t="inlineStr">
         <is>
-          <t>2010-07-29</t>
+          <t>2009-09-08</t>
         </is>
       </c>
       <c r="Z36" s="1" t="inlineStr">
@@ -5687,12 +5687,12 @@
       </c>
       <c r="X37" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="Y37" s="1" t="inlineStr">
         <is>
-          <t>2010-08-03</t>
+          <t>2008-09-11</t>
         </is>
       </c>
       <c r="Z37" s="1" t="inlineStr">
@@ -5839,12 +5839,12 @@
       </c>
       <c r="X38" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>5.56</t>
         </is>
       </c>
       <c r="Y38" s="1" t="inlineStr">
         <is>
-          <t>2011-04-27</t>
+          <t>2010-06-07</t>
         </is>
       </c>
       <c r="Z38" s="1" t="inlineStr">
@@ -5991,12 +5991,12 @@
       </c>
       <c r="X39" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y39" s="1" t="inlineStr">
         <is>
-          <t>2010-10-18</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z39" s="1" t="inlineStr">
@@ -6295,12 +6295,12 @@
       </c>
       <c r="X41" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y41" s="1" t="inlineStr">
         <is>
-          <t>2010-10-20</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z41" s="1" t="inlineStr">
@@ -6447,12 +6447,12 @@
       </c>
       <c r="X42" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="Y42" s="1" t="inlineStr">
         <is>
-          <t>2010-10-21</t>
+          <t>2009-03-06</t>
         </is>
       </c>
       <c r="Z42" s="1" t="inlineStr">
@@ -6599,12 +6599,12 @@
       </c>
       <c r="X43" s="1" t="inlineStr">
         <is>
-          <t>2.28</t>
+          <t>2.74</t>
         </is>
       </c>
       <c r="Y43" s="1" t="inlineStr">
         <is>
-          <t>2011-04-21</t>
+          <t>2009-09-14</t>
         </is>
       </c>
       <c r="Z43" s="1" t="inlineStr">
@@ -6751,12 +6751,12 @@
       </c>
       <c r="X44" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="Y44" s="1" t="inlineStr">
         <is>
-          <t>2010-06-03</t>
+          <t>2008-09-17</t>
         </is>
       </c>
       <c r="Z44" s="1" t="inlineStr">
@@ -7027,12 +7027,12 @@
       </c>
       <c r="X46" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="Y46" s="1" t="inlineStr">
         <is>
-          <t>2010-06-02</t>
+          <t>2007-12-06</t>
         </is>
       </c>
       <c r="Z46" s="1" t="inlineStr">
@@ -7163,7 +7163,7 @@
       </c>
       <c r="X47" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="Y47" s="1" t="inlineStr">
@@ -7315,12 +7315,12 @@
       </c>
       <c r="X48" s="1" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Y48" s="1" t="inlineStr">
         <is>
-          <t>2010-06-02</t>
+          <t>No Detect Data</t>
         </is>
       </c>
       <c r="Z48" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Made some changes to getWatershed to correct Mortandad, applied those changes throughout process. Updated tablesToExcel to write a separate section for LA and Paj canyons.
</commit_message>
<xml_diff>
--- a/Tables/Alluvial- Appendix.xlsx
+++ b/Tables/Alluvial- Appendix.xlsx
@@ -1231,7 +1231,7 @@
       </c>
       <c r="P6" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q6" s="1" t="inlineStr">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="P7" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q7" s="1" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="P8" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q8" s="1" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="P9" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q9" s="1" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="P10" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q10" s="1" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="P11" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q11" s="1" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="P12" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q12" s="1" t="inlineStr">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="P13" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q13" s="1" t="inlineStr">
@@ -2391,7 +2391,7 @@
       </c>
       <c r="P14" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q14" s="1" t="inlineStr">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="P15" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q15" s="1" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="P16" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q16" s="1" t="inlineStr">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="P17" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q17" s="1" t="inlineStr">
@@ -2959,7 +2959,7 @@
       </c>
       <c r="P18" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q18" s="1" t="inlineStr">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="P19" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q19" s="1" t="inlineStr">
@@ -3235,7 +3235,7 @@
       </c>
       <c r="P20" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q20" s="1" t="inlineStr">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="P21" s="1" t="inlineStr">
         <is>
-          <t>Mortendad</t>
+          <t>Mortandad</t>
         </is>
       </c>
       <c r="Q21" s="1" t="inlineStr">
@@ -8248,7 +8248,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8258,7 +8258,7 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="12.25"/>
     <col customWidth="1" max="2" min="2" width="10.14"/>
-    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="3" min="3" width="13"/>
     <col customWidth="1" max="4" min="4" width="9.15"/>
     <col customWidth="1" max="5" min="5" width="7"/>
     <col customWidth="1" max="6" min="6" width="16.25"/>
@@ -8494,7 +8494,7 @@
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Mortendad Canyon</t>
+          <t>Mortandad Canyon</t>
         </is>
       </c>
       <c r="H8" s="5" t="n"/>
@@ -9174,7 +9174,7 @@
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Los Alamos and Pajarito Canyons</t>
+          <t>Los Alamos Canyon</t>
         </is>
       </c>
       <c r="H25" s="5" t="n"/>
@@ -9936,230 +9936,196 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>18-BG-1</t>
-        </is>
-      </c>
-      <c r="B44" s="1" t="inlineStr">
-        <is>
-          <t>35.84426</t>
-        </is>
-      </c>
-      <c r="C44" s="1" t="inlineStr">
-        <is>
-          <t>-106.27114</t>
-        </is>
-      </c>
-      <c r="D44" s="1" t="inlineStr">
-        <is>
-          <t>9/1/94</t>
-        </is>
-      </c>
-      <c r="E44" s="1" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="F44" s="1" t="inlineStr">
-        <is>
-          <t>10 - 35</t>
-        </is>
-      </c>
-      <c r="G44" s="1" t="inlineStr">
-        <is>
-          <t>6.72</t>
-        </is>
-      </c>
-      <c r="H44" s="1" t="inlineStr">
-        <is>
-          <t>2/22/10</t>
-        </is>
-      </c>
+      <c r="A44" s="4" t="inlineStr">
+        <is>
+          <t>Pajarito Canyon</t>
+        </is>
+      </c>
+      <c r="H44" s="5" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>18-MW-11</t>
+          <t>18-BG-1</t>
         </is>
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>35.84031</t>
+          <t>35.84426</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr">
         <is>
-          <t>-106.2649</t>
-        </is>
-      </c>
-      <c r="D45" s="1" t="inlineStr"/>
+          <t>-106.27114</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>9/1/94</t>
+        </is>
+      </c>
       <c r="E45" s="1" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>27 - 47</t>
+          <t>10 - 35</t>
         </is>
       </c>
       <c r="G45" s="1" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>6.72</t>
         </is>
       </c>
       <c r="H45" s="1" t="inlineStr">
         <is>
-          <t>6/17/08</t>
+          <t>2/22/10</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>18-MW-8</t>
+          <t>18-MW-11</t>
         </is>
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>35.83899</t>
+          <t>35.84031</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr">
         <is>
-          <t>-106.26924</t>
-        </is>
-      </c>
-      <c r="D46" s="1" t="inlineStr">
-        <is>
-          <t>8/4/94</t>
-        </is>
-      </c>
+          <t>-106.2649</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="inlineStr"/>
       <c r="E46" s="1" t="inlineStr">
         <is>
-          <t>37.9</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>8 - 38</t>
+          <t>27 - 47</t>
         </is>
       </c>
       <c r="G46" s="1" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="H46" s="1" t="inlineStr">
         <is>
-          <t>6/16/08</t>
+          <t>6/17/08</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>18-MW-9</t>
+          <t>18-MW-8</t>
         </is>
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>35.83964</t>
+          <t>35.83899</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr">
         <is>
-          <t>-106.26507</t>
+          <t>-106.26924</t>
         </is>
       </c>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>7/21/94</t>
+          <t>8/4/94</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>37.9</t>
         </is>
       </c>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>6 - 21</t>
+          <t>8 - 38</t>
         </is>
       </c>
       <c r="G47" s="1" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="H47" s="1" t="inlineStr">
         <is>
-          <t>12/11/06</t>
+          <t>6/16/08</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>3MAO-2</t>
+          <t>18-MW-9</t>
         </is>
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>35.83915</t>
+          <t>35.83964</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr">
         <is>
-          <t>-106.27238</t>
+          <t>-106.26507</t>
         </is>
       </c>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>6/4/08</t>
+          <t>7/21/94</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>14.7 - 24.7</t>
+          <t>6 - 21</t>
         </is>
       </c>
       <c r="G48" s="1" t="inlineStr">
         <is>
-          <t>5.56</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="H48" s="1" t="inlineStr">
         <is>
-          <t>6/7/10</t>
+          <t>12/11/06</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>PCAO-5</t>
+          <t>3MAO-2</t>
         </is>
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>35.85353</t>
+          <t>35.83915</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr">
         <is>
-          <t>-106.29474</t>
+          <t>-106.27238</t>
         </is>
       </c>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>5/3/08</t>
+          <t>6/4/08</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr">
@@ -10174,118 +10140,118 @@
       </c>
       <c r="G49" s="1" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>5.56</t>
         </is>
       </c>
       <c r="H49" s="1" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>6/7/10</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>PCAO-6</t>
+          <t>PCAO-5</t>
         </is>
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>35.85336</t>
+          <t>35.85353</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr">
         <is>
-          <t>-106.29322</t>
+          <t>-106.29474</t>
         </is>
       </c>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>6/5/08</t>
+          <t>5/3/08</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>8 - 15</t>
+          <t>14.7 - 24.7</t>
         </is>
       </c>
       <c r="G50" s="1" t="inlineStr">
         <is>
-          <t>2.68</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H50" s="1" t="inlineStr">
         <is>
-          <t>6/4/10</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>PCAO-7a</t>
+          <t>PCAO-6</t>
         </is>
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>35.83869</t>
+          <t>35.85336</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr">
         <is>
-          <t>-106.26174</t>
+          <t>-106.29322</t>
         </is>
       </c>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>5/30/08</t>
+          <t>6/5/08</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>9.7 - 19.7</t>
+          <t>8 - 15</t>
         </is>
       </c>
       <c r="G51" s="1" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="H51" s="1" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>6/4/10</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>PCAO-7b2</t>
+          <t>PCAO-7a</t>
         </is>
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>35.8385</t>
+          <t>35.83869</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr">
         <is>
-          <t>-106.26205</t>
+          <t>-106.26174</t>
         </is>
       </c>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>5/27/08</t>
+          <t>5/30/08</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr">
@@ -10295,39 +10261,39 @@
       </c>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>10 - 20</t>
+          <t>9.7 - 19.7</t>
         </is>
       </c>
       <c r="G52" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="H52" s="1" t="inlineStr">
         <is>
-          <t>12/18/08</t>
+          <t>NA</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>PCAO-7c</t>
+          <t>PCAO-7b2</t>
         </is>
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>35.8381</t>
+          <t>35.8385</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr">
         <is>
-          <t>-106.26252</t>
+          <t>-106.26205</t>
         </is>
       </c>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>5/16/08</t>
+          <t>5/27/08</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr">
@@ -10337,118 +10303,118 @@
       </c>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>9.7 - 19.7</t>
+          <t>10 - 20</t>
         </is>
       </c>
       <c r="G53" s="1" t="inlineStr">
         <is>
-          <t>2.74</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H53" s="1" t="inlineStr">
         <is>
-          <t>9/14/09</t>
+          <t>12/18/08</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>PCAO-9</t>
+          <t>PCAO-7c</t>
         </is>
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>35.82614</t>
+          <t>35.8381</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr">
         <is>
-          <t>-106.23271</t>
+          <t>-106.26252</t>
         </is>
       </c>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>6/12/08</t>
+          <t>5/16/08</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>6 - 16</t>
+          <t>9.7 - 19.7</t>
         </is>
       </c>
       <c r="G54" s="1" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>2.74</t>
         </is>
       </c>
       <c r="H54" s="1" t="inlineStr">
         <is>
-          <t>9/17/08</t>
+          <t>9/14/09</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>PCO-1</t>
+          <t>PCAO-9</t>
         </is>
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>35.83716</t>
+          <t>35.82614</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr">
         <is>
-          <t>-106.25843</t>
+          <t>-106.23271</t>
         </is>
       </c>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>6/30/85</t>
+          <t>6/12/08</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>4 - 12</t>
+          <t>6 - 16</t>
         </is>
       </c>
       <c r="G55" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H55" s="1" t="inlineStr">
         <is>
-          <t>8/24/05</t>
+          <t>9/17/08</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>PCO-2</t>
+          <t>PCO-1</t>
         </is>
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>35.83016</t>
+          <t>35.83716</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr">
         <is>
-          <t>-106.24567</t>
+          <t>-106.25843</t>
         </is>
       </c>
       <c r="D56" s="1" t="inlineStr">
@@ -10458,39 +10424,39 @@
       </c>
       <c r="E56" s="1" t="inlineStr">
         <is>
-          <t>9.5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>1.5 - 9.5</t>
+          <t>4 - 12</t>
         </is>
       </c>
       <c r="G56" s="1" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H56" s="1" t="inlineStr">
         <is>
-          <t>6/25/07</t>
+          <t>8/24/05</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>PCO-3</t>
+          <t>PCO-2</t>
         </is>
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>35.82479</t>
+          <t>35.83016</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr">
         <is>
-          <t>-106.23087</t>
+          <t>-106.24567</t>
         </is>
       </c>
       <c r="D57" s="1" t="inlineStr">
@@ -10500,73 +10466,116 @@
       </c>
       <c r="E57" s="1" t="inlineStr">
         <is>
-          <t>17.7</t>
+          <t>9.5</t>
         </is>
       </c>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>5.7 - 17.7</t>
+          <t>1.5 - 9.5</t>
         </is>
       </c>
       <c r="G57" s="1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="H57" s="1" t="inlineStr">
         <is>
-          <t>12/7/07</t>
+          <t>6/25/07</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
+          <t>PCO-3</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>35.82479</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>-106.23087</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>6/30/85</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>17.7</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>5.7 - 17.7</t>
+        </is>
+      </c>
+      <c r="G58" s="1" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="H58" s="1" t="inlineStr">
+        <is>
+          <t>12/7/07</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
           <t>TMO-1</t>
         </is>
       </c>
-      <c r="B58" s="1" t="inlineStr">
+      <c r="B59" s="1" t="inlineStr">
         <is>
           <t>35.8541</t>
         </is>
       </c>
-      <c r="C58" s="1" t="inlineStr">
+      <c r="C59" s="1" t="inlineStr">
         <is>
           <t>-106.29585</t>
         </is>
       </c>
-      <c r="D58" s="1" t="inlineStr">
+      <c r="D59" s="1" t="inlineStr">
         <is>
           <t>6/9/08</t>
         </is>
       </c>
-      <c r="E58" s="1" t="inlineStr">
+      <c r="E59" s="1" t="inlineStr">
         <is>
           <t>6.5</t>
         </is>
       </c>
-      <c r="F58" s="1" t="inlineStr">
+      <c r="F59" s="1" t="inlineStr">
         <is>
           <t>3.5 - 6.5</t>
         </is>
       </c>
-      <c r="G58" s="1" t="inlineStr">
+      <c r="G59" s="1" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="H58" s="1" t="inlineStr">
+      <c r="H59" s="1" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A44:H44"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>